<commit_message>
update the last changes
</commit_message>
<xml_diff>
--- a/Módulo 3/Limpeza e transformação de dados/categorias_pivot.xlsx
+++ b/Módulo 3/Limpeza e transformação de dados/categorias_pivot.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/442e7cdbf85a6b61/Documentos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/442e7cdbf85a6b61/Documentos/GitHub/power_bi_analyst/Módulo 3/Limpeza e transformação de dados/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EFA5D80F-CB50-4672-9AD2-ECB47500BEB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="8_{EFA5D80F-CB50-4672-9AD2-ECB47500BEB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D0D35705-3840-4BC4-B8B4-C58D8E13FFC1}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="1440" windowWidth="20730" windowHeight="11760" xr2:uid="{A539DBCC-EA73-426F-8517-60D8749DB301}"/>
+    <workbookView xWindow="-20610" yWindow="1440" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{A539DBCC-EA73-426F-8517-60D8749DB301}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Vendas" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="25">
   <si>
     <t>Categoria</t>
   </si>
@@ -108,6 +109,9 @@
   </si>
   <si>
     <t>pneu aro 25</t>
+  </si>
+  <si>
+    <t>Total vendido</t>
   </si>
 </sst>
 </file>
@@ -461,8 +465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{953B9B81-1985-44F8-972A-C33F9B990AE1}">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17:B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -628,7 +632,153 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1684EE0-5484-4B79-8A0F-FD4FE67B36C0}">
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.77734375" customWidth="1"/>
+    <col min="2" max="2" width="12.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>235.12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>700.23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>569.23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14">
+        <v>300</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D261F867CE82EA489D88415C5AC993C4" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="98bb77bb0cc12de918e03a1e3cd5cdf6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="3019d89f-f031-4d1e-b7d8-a3aff2a03c55" xmlns:ns4="878716db-020a-4087-b0dc-18eb9c1797a2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cc9d484427f0d9d16fc0d56f57f5cb3c" ns3:_="" ns4:_="">
     <xsd:import namespace="3019d89f-f031-4d1e-b7d8-a3aff2a03c55"/>
@@ -851,22 +1001,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC95A492-758A-4A4D-A566-804A7A4FB5AE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="3019d89f-f031-4d1e-b7d8-a3aff2a03c55"/>
+    <ds:schemaRef ds:uri="878716db-020a-4087-b0dc-18eb9c1797a2"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0420D13F-D520-4642-8575-65D40708622A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3F426105-CD30-4D7A-921C-26C87475E2D6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -883,29 +1043,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0420D13F-D520-4642-8575-65D40708622A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC95A492-758A-4A4D-A566-804A7A4FB5AE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="3019d89f-f031-4d1e-b7d8-a3aff2a03c55"/>
-    <ds:schemaRef ds:uri="878716db-020a-4087-b0dc-18eb9c1797a2"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>